<commit_message>
Added Tasks, dates and assignments
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8520" windowHeight="2920" xr2:uid="{0FA9E7B1-238D-4313-9882-BAC7D8C03296}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{0FA9E7B1-238D-4313-9882-BAC7D8C03296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -51,14 +51,96 @@
   </si>
   <si>
     <t>Target End Date</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Milestone 2 Rough Draft 1</t>
+  </si>
+  <si>
+    <t>Milestone 2 Rough Draft 2</t>
+  </si>
+  <si>
+    <t>Milestone 2 Rough Draft 3</t>
+  </si>
+  <si>
+    <t>Milestone 2 Final</t>
+  </si>
+  <si>
+    <t>Create GIT repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2700-Indu</t>
+  </si>
+  <si>
+    <t>Create Project Plan</t>
+  </si>
+  <si>
+    <t>Create Change Log</t>
+  </si>
+  <si>
+    <t>2700-Indu</t>
+  </si>
+  <si>
+    <t>Research Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2100-Prerana </t>
+  </si>
+  <si>
+    <t>2100-Prerana</t>
+  </si>
+  <si>
+    <t>Milestone 1 Deliverable 1</t>
+  </si>
+  <si>
+    <t>Milestone 1 Deliverable 2</t>
+  </si>
+  <si>
+    <t>Milestone 1 Deliverable 3</t>
+  </si>
+  <si>
+    <t>Milestone 1 Deliverable 4</t>
+  </si>
+  <si>
+    <t>Milestone 1 Deliverable 5</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Milestone 3 Rough Draft 1</t>
+  </si>
+  <si>
+    <t>Milestone 3 Rough Draft 2</t>
+  </si>
+  <si>
+    <t>Milestone 3 Final</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Milestone 4</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>Milestone 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0;[Red]0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -110,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -118,9 +200,18 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,25 +526,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE75DE5-79E2-42E1-845C-3FD67C7890B7}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="8.7265625" style="12"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
     <col min="4" max="5" width="15.1796875" style="6" customWidth="1"/>
     <col min="6" max="6" width="19.7265625" style="6" customWidth="1"/>
     <col min="7" max="7" width="14.453125" style="6" customWidth="1"/>
     <col min="8" max="8" width="16.81640625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="9" max="9" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -482,205 +574,457 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E2" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F2" s="5">
+        <v>43142</v>
+      </c>
+      <c r="G2" s="5">
+        <v>43142</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="3"/>
+      <c r="A3" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43144</v>
+      </c>
+      <c r="G3" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="3"/>
+      <c r="A4" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43144</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="3"/>
+      <c r="A5" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43144</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="3"/>
+      <c r="A6" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F6" s="5">
+        <v>43144</v>
+      </c>
+      <c r="G6" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="3"/>
+      <c r="A7" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F7" s="5">
+        <v>43144</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="3"/>
+      <c r="A8" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43143</v>
+      </c>
+      <c r="G8" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="3"/>
+      <c r="A9" s="11">
+        <v>1.7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F9" s="5">
+        <v>43143</v>
+      </c>
+      <c r="G9" s="5">
+        <v>43144</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43147</v>
+      </c>
+      <c r="F10" s="5">
+        <v>43143</v>
+      </c>
+      <c r="G10" s="5">
+        <v>43143</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43144</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43151</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="8"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5">
+        <v>43151</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43158</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="8"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5">
+        <v>43158</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43165</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="8"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5">
+        <v>43165</v>
+      </c>
+      <c r="E14" s="5">
+        <v>43172</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="8"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="11">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5">
+        <v>43193</v>
+      </c>
+      <c r="E15" s="5">
+        <v>43200</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="8"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="11">
+        <v>3.1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5">
+        <v>43200</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43207</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="11">
+        <v>3.2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="5">
+        <v>43207</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43214</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="8"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="11">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="5">
+        <v>43221</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43228</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="8"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="A19" s="11">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="5">
+        <v>43137</v>
+      </c>
+      <c r="E19" s="5">
+        <v>43228</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="8"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="5"/>
@@ -691,7 +1035,7 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="5"/>
@@ -702,7 +1046,7 @@
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="5"/>
@@ -713,7 +1057,7 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="5"/>
@@ -724,7 +1068,7 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="5"/>
@@ -735,7 +1079,7 @@
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="5"/>
@@ -745,6 +1089,94 @@
       <c r="H25" s="8"/>
       <c r="I25" s="3"/>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="11"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>